<commit_message>
CCDR Japan Data Only
</commit_message>
<xml_diff>
--- a/Data/Raw/First_Draft_Cleaned_CCDR.xlsx
+++ b/Data/Raw/First_Draft_Cleaned_CCDR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benculberson/Documents/Duke /Spring 2022/Environmental Data Analytics/Shapiro_DeAngeli_Culberson_ENV872_EDA_FinalProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benculberson/Documents/Duke /Spring 2022/Environmental Data Analytics/Shapiro_DeAngeli_Culberson_ENV872_EDA_FinalProject/Data/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1F30F4C1-66E7-1645-82B2-7CC69801B152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{11F14345-6B99-3E40-86C6-69A6CFBC23E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="47040" windowHeight="19960" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="First Draft Cleaned CCDR" sheetId="1" r:id="rId1"/>

</xml_diff>